<commit_message>
060125 EOD Tested Goods Receipt and NTA AP Invoice
</commit_message>
<xml_diff>
--- a/Daily Activity/2024/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024/2024 Work Sheet.xlsx
@@ -778,7 +778,7 @@
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1124,7 +1124,7 @@
       <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1841,18 +1841,18 @@
   </sheetPr>
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.83"/>
@@ -2628,7 +2628,7 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">

</xml_diff>

<commit_message>
100125 EOD completed ACL Documentation for a user
</commit_message>
<xml_diff>
--- a/Daily Activity/2024/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024/2024 Work Sheet.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Oct-10" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Nov-11" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Dec-12" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Summary" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="2024 Summary" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Dec-12'!$A$1:$W$33</definedName>
@@ -778,7 +778,7 @@
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1124,7 +1124,7 @@
       <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1841,13 +1841,13 @@
   </sheetPr>
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -2624,11 +2624,11 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">

</xml_diff>

<commit_message>
130125 EOD Completed 185 SR in Accounting ACL
</commit_message>
<xml_diff>
--- a/Daily Activity/2024/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024/2024 Work Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Oct-10" sheetId="1" state="visible" r:id="rId2"/>
@@ -435,7 +435,7 @@
     <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -464,6 +464,17 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -475,7 +486,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66BAAA"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF729FCF"/>
       </patternFill>
     </fill>
     <fill>
@@ -486,8 +497,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4C7DC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF66BAAA"/>
       </patternFill>
     </fill>
   </fills>
@@ -560,7 +571,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,15 +668,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,9 +733,9 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -772,13 +795,13 @@
   </sheetPr>
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1118,13 +1141,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1841,13 +1864,13 @@
   </sheetPr>
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B22" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -2622,134 +2645,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="F5:K19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="G5" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="H5" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="I5" s="24" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="26" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="26" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="26" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="26" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="26" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="26" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="26" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="G15" s="28" t="n">
         <f aca="false">COUNTIF('Oct-10'!J2:J32,"YES")</f>
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="H15" s="27" t="n">
         <f aca="false">COUNTIF('Oct-10'!K2:K32,"YES")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="I15" s="28" t="n">
+        <f aca="false">SUM('Oct-10'!I2:I30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="G16" s="28" t="n">
         <f aca="false">COUNTIF('Nov-11'!B2:B31,"YES")</f>
         <v>6</v>
       </c>
-      <c r="C12" s="25" t="n">
+      <c r="H16" s="28" t="n">
         <f aca="false">COUNTIF('Nov-11'!C2:C32,"YES")</f>
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="I16" s="28" t="n">
         <f aca="false">SUM('Nov-11'!I2:I30)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="25" t="n">
+      <c r="G17" s="28" t="n">
         <f aca="false">COUNTIF('Dec-12'!B2:B31,"YES")</f>
         <v>7</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="H17" s="27" t="n">
         <f aca="false">COUNTIF('Dec-12'!C2:C32,"YES")</f>
         <v>0</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="I17" s="27" t="n">
         <f aca="false">SUM('Dec-12'!J2:J30)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="26" t="n">
-        <f aca="false">SUM(B2:B13)</f>
+      <c r="G19" s="29" t="n">
+        <f aca="false">SUM(G6:G17)</f>
         <v>15</v>
       </c>
-      <c r="C15" s="26" t="n">
-        <f aca="false">SUM(C2:C13)</f>
+      <c r="H19" s="29" t="n">
+        <f aca="false">SUM(H6:H17)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="26" t="n">
-        <f aca="false">SUM(D2:D13)</f>
+      <c r="I19" s="29" t="n">
+        <f aca="false">SUM(I6:I17)</f>
         <v>36</v>
       </c>
     </row>

</xml_diff>